<commit_message>
pipeline added training and inference
</commit_message>
<xml_diff>
--- a/artifacts/model_evaluation/metrics.xlsx
+++ b/artifacts/model_evaluation/metrics.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -630,6 +630,37 @@
         <v>0.005993775805763789</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-10-24 14:45:28</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9985354969052938</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.00807231991497321</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0001208275992999146</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.01099216081122882</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9871104351019552</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.003673089070717696</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.688071937762312e-05</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.006072949808587513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>